<commit_message>
bugs in english sample fixed
</commit_message>
<xml_diff>
--- a/sample_apps/network_en/sample-knowledge-en.xlsx
+++ b/sample_apps/network_en/sample-knowledge-en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb-develop\sample_apps\network_en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99FA996-1AE2-4DD2-BFA1-5A1AF3BA606B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F365935-A1A8-4D6F-8FFD-39E4EAFA5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -68,10 +68,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>slot</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Hello! I'm a chatbot. Let me ask you about sandwich. Do you have sandwiches very often?</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -170,10 +166,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>synonyms</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -350,9 +342,6 @@
     <t>_set(&amp;topic_sandwich,#favorite-sandwich)</t>
   </si>
   <si>
-    <t>is_novel_sandwith(#favorite-sandwich)</t>
-  </si>
-  <si>
     <t>egg-salad-sandwich</t>
   </si>
   <si>
@@ -361,6 +350,18 @@
   </si>
   <si>
     <t>known-sandwich</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>slot name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>entity class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>is_novel_sandwich(#favorite-sandwich)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -786,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -797,8 +798,7 @@
     <col min="3" max="3" width="36.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="40.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="46.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.625" style="4"/>
   </cols>
@@ -808,244 +808,244 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1082,90 +1082,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1193,18 +1193,18 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1234,30 +1234,30 @@
         <v>2</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1274,13 +1274,13 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" style="7"/>
-    <col min="2" max="2" width="9.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.25" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="7"/>
@@ -1291,129 +1291,129 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bug in whitespace_tokenizer fixed
</commit_message>
<xml_diff>
--- a/sample_apps/network_en/sample-knowledge-en.xlsx
+++ b/sample_apps/network_en/sample-knowledge-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.3\sample_apps\network_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F365935-A1A8-4D6F-8FFD-39E4EAFA5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8311966-042A-4681-B20D-45C14BF52CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
commas and semicolons in constants in scenario functions allowd
</commit_message>
<xml_diff>
--- a/sample_apps/network_en/sample-knowledge-en.xlsx
+++ b/sample_apps/network_en/sample-knowledge-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.3\sample_apps\network_en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8311966-042A-4681-B20D-45C14BF52CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EAD2B2-B0C6-4FE2-B68C-68125667AC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -330,12 +330,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_eq(#favorite-sandwich, "egg salad sandwich")</t>
-  </si>
-  <si>
-    <t>_set(&amp;topic_sandwich, #favorite-sandwich)</t>
-  </si>
-  <si>
     <t>is_known_sandwich(#favorite-sandwich)</t>
   </si>
   <si>
@@ -362,6 +356,14 @@
   </si>
   <si>
     <t>is_novel_sandwich(#favorite-sandwich)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_set(&amp;topic_sandwich, "egg salad sandwich")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_eq(#favorite-sandwich, "egg salad, sandwich")</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -787,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -927,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
@@ -948,13 +950,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
@@ -968,7 +970,7 @@
         <v>23</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>25</v>
@@ -998,7 +1000,7 @@
     </row>
     <row r="13" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>62</v>
@@ -1012,7 +1014,7 @@
     </row>
     <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>63</v>
@@ -1059,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1193,10 +1195,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -1234,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>57</v>
@@ -1291,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>5</v>

</xml_diff>